<commit_message>
update excel id card
</commit_message>
<xml_diff>
--- a/src/main/resources/excel-template/template-annual.xlsx
+++ b/src/main/resources/excel-template/template-annual.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pele/job/icoop-cm/icoop-backend/src/main/resources/excel-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B3145BE-63B3-B743-97B7-02BF5310F32D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8548B5-F138-8C42-82C2-CB95663C4424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36000" yWindow="5900" windowWidth="38400" windowHeight="18640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36000" yWindow="5900" windowWidth="38400" windowHeight="18640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="รายชื่อสมาชิกที่คงอยู่" sheetId="1" r:id="rId1"/>
@@ -125,7 +125,7 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">jx:area(lastCell="E2")
+          <t xml:space="preserve">jx:area(lastCell="F2")
 </t>
         </r>
         <r>
@@ -153,7 +153,7 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t>" var="data" varIndex="index" lastCell="E2")</t>
+          <t>" var="data" varIndex="index" lastCell="F2")</t>
         </r>
       </text>
     </comment>
@@ -162,7 +162,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
   <si>
     <t>ลำดับ</t>
   </si>
@@ -204,6 +204,12 @@
   </si>
   <si>
     <t>${index + 1}</t>
+  </si>
+  <si>
+    <t>เลขบัตรประชาชน</t>
+  </si>
+  <si>
+    <t>${data.idCard}</t>
   </si>
 </sst>
 </file>
@@ -358,7 +364,48 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="31">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="TH SarabunPSK"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1229,42 +1276,43 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D2" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D2" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <autoFilter ref="A1:D2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="ลำดับ" dataDxfId="24"/>
-    <tableColumn id="24" xr3:uid="{84E55B6A-3159-B54D-8F73-C23615212DFD}" name="หน่วยงาน" dataDxfId="23"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="รหัสพนักงาน" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ชื่อพนักงาน" dataDxfId="21"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="ลำดับ" dataDxfId="25"/>
+    <tableColumn id="24" xr3:uid="{84E55B6A-3159-B54D-8F73-C23615212DFD}" name="หน่วยงาน" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="รหัสพนักงาน" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ชื่อพนักงาน" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7A2AFCCC-2821-AE43-8B79-857E16535308}" name="Table14" displayName="Table14" ref="A1:F2" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7A2AFCCC-2821-AE43-8B79-857E16535308}" name="Table14" displayName="Table14" ref="A1:F2" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18" totalsRowBorderDxfId="17">
   <autoFilter ref="A1:F2" xr:uid="{7A2AFCCC-2821-AE43-8B79-857E16535308}"/>
   <tableColumns count="6">
-    <tableColumn id="10" xr3:uid="{D2F6A2CF-5BD2-814C-A5B8-92A57F4BDD05}" name="ลำดับ" dataDxfId="15"/>
-    <tableColumn id="24" xr3:uid="{AC1A5815-EEC6-A646-A4D9-14035955CD2D}" name="หน่วยงาน" dataDxfId="14"/>
-    <tableColumn id="1" xr3:uid="{B633C69A-6BB6-3A40-8678-AC1616D27231}" name="รหัสพนักงาน" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{95FD2B1A-1BFB-DA4F-91B8-613D6418B396}" name="ชื่อพนักงาน" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{3830FE34-A50E-9546-8203-E9ED8A560E66}" name="สาเหตุ" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{BEB6DAB4-99E2-6442-8604-EFF0D2B59848}" name="เดือนลาออก" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{D2F6A2CF-5BD2-814C-A5B8-92A57F4BDD05}" name="ลำดับ" dataDxfId="16"/>
+    <tableColumn id="24" xr3:uid="{AC1A5815-EEC6-A646-A4D9-14035955CD2D}" name="หน่วยงาน" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{B633C69A-6BB6-3A40-8678-AC1616D27231}" name="รหัสพนักงาน" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{95FD2B1A-1BFB-DA4F-91B8-613D6418B396}" name="ชื่อพนักงาน" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{3830FE34-A50E-9546-8203-E9ED8A560E66}" name="สาเหตุ" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{BEB6DAB4-99E2-6442-8604-EFF0D2B59848}" name="เดือนลาออก" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D84347FB-B30A-2F4D-BCE4-F8F1AFC9785B}" name="Table143" displayName="Table143" ref="A1:E2" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
-  <autoFilter ref="A1:E2" xr:uid="{D84347FB-B30A-2F4D-BCE4-F8F1AFC9785B}"/>
-  <tableColumns count="5">
-    <tableColumn id="10" xr3:uid="{D7EF2533-4C58-CB47-AF22-CFEE621ED660}" name="ลำดับ" dataDxfId="4"/>
-    <tableColumn id="24" xr3:uid="{C5ED4D82-CFC7-8C4F-A530-A710F4CACC2B}" name="หน่วยงาน" dataDxfId="3"/>
-    <tableColumn id="1" xr3:uid="{D51296F6-87B8-C54A-A84D-C30522CEDF0B}" name="รหัสพนักงาน" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{160FD14E-447B-094A-A292-BE4781A7BE35}" name="ชื่อพนักงาน" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{8038C63D-D1C8-B44D-B095-5F457C157369}" name="เดือนที่สมัคร" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D84347FB-B30A-2F4D-BCE4-F8F1AFC9785B}" name="Table143" displayName="Table143" ref="A1:F2" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+  <autoFilter ref="A1:F2" xr:uid="{D84347FB-B30A-2F4D-BCE4-F8F1AFC9785B}"/>
+  <tableColumns count="6">
+    <tableColumn id="10" xr3:uid="{D7EF2533-4C58-CB47-AF22-CFEE621ED660}" name="ลำดับ" dataDxfId="5"/>
+    <tableColumn id="24" xr3:uid="{C5ED4D82-CFC7-8C4F-A530-A710F4CACC2B}" name="หน่วยงาน" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{D51296F6-87B8-C54A-A84D-C30522CEDF0B}" name="รหัสพนักงาน" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{160FD14E-447B-094A-A292-BE4781A7BE35}" name="ชื่อพนักงาน" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{73BE3F1F-F7F2-8C4B-AA74-DF12A9FC1222}" name="เลขบัตรประชาชน" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{8038C63D-D1C8-B44D-B095-5F457C157369}" name="เดือนที่สมัคร" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1569,7 +1617,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D861"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -2548,9 +2596,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ABF30E1-7399-464C-8173-F56C98B42388}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24"/>
   <cols>
@@ -2558,10 +2608,11 @@
     <col min="2" max="2" width="49.6640625" style="7" customWidth="1"/>
     <col min="3" max="3" width="25" style="7" customWidth="1"/>
     <col min="4" max="4" width="38.6640625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="24.83203125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="26.83203125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" ht="25" customHeight="1">
+    <row r="1" spans="1:6" s="3" customFormat="1" ht="25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2575,10 +2626,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="3" customFormat="1" ht="25" customHeight="1">
+    <row r="2" spans="1:6" s="3" customFormat="1" ht="25" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
@@ -2591,7 +2645,10 @@
       <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>